<commit_message>
se realiza insercion de cuentas y validacion de usuarios y cuentas
</commit_message>
<xml_diff>
--- a/DatosUsuario.xlsx
+++ b/DatosUsuario.xlsx
@@ -12,45 +12,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
-  <si>
-    <t>Dirección</t>
-  </si>
-  <si>
-    <t>Teléfono</t>
-  </si>
-  <si>
-    <t>Correo Electrónico</t>
-  </si>
-  <si>
-    <t>Ocupación</t>
-  </si>
-  <si>
-    <t>Ingresos Mensuales</t>
-  </si>
-  <si>
-    <t>tkg</t>
-  </si>
-  <si>
-    <t>ktgt</t>
-  </si>
-  <si>
-    <t>itkktk</t>
-  </si>
-  <si>
-    <t>tgkkjotm</t>
-  </si>
-  <si>
-    <t/>
+    <t>ingresos</t>
+  </si>
+  <si>
+    <t>apellido</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>ocupacion</t>
+  </si>
+  <si>
+    <t>dpi</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t>guatemala</t>
+  </si>
+  <si>
+    <t>estudiante</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>123466</t>
   </si>
 </sst>
 </file>
@@ -95,20 +110,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="3.80859375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="8.39453125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="9.4375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="8.953125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.67578125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="10.54296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="18.68359375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="2.9453125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.4765625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.171875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.15625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.484375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5859375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.7265625"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.6171875"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="8.12890625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -136,10 +152,13 @@
       <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
+      <c r="I1" t="s" s="0">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>8</v>
+      <c r="A2" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>9</v>
@@ -154,13 +173,103 @@
         <v>12</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se realiza actualizacion de cliente
</commit_message>
<xml_diff>
--- a/DatosUsuario.xlsx
+++ b/DatosUsuario.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>123466</t>
+  </si>
+  <si>
+    <t>profesor</t>
+  </si>
+  <si>
+    <t>maestro</t>
   </si>
 </sst>
 </file>
@@ -173,7 +179,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s" s="0">
         <v>14</v>

</xml_diff>